<commit_message>
Template done 9 May
</commit_message>
<xml_diff>
--- a/dss/PyomoSolver/case_data.xlsx
+++ b/dss/PyomoSolver/case_data.xlsx
@@ -12,15 +12,17 @@
     <sheet name="industry" sheetId="3" r:id="rId3"/>
     <sheet name="industry_supply" sheetId="4" r:id="rId4"/>
     <sheet name="industry_demand" sheetId="5" r:id="rId5"/>
-    <sheet name="feasible" sheetId="6" r:id="rId6"/>
-    <sheet name="distance" sheetId="7" r:id="rId7"/>
+    <sheet name="investment_demand" sheetId="6" r:id="rId6"/>
+    <sheet name="invest_cost" sheetId="7" r:id="rId7"/>
+    <sheet name="feasible" sheetId="8" r:id="rId8"/>
+    <sheet name="distance" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
   <si>
     <t>material</t>
   </si>
@@ -31,6 +33,15 @@
     <t>entity</t>
   </si>
   <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
     <t>company</t>
   </si>
   <si>
@@ -46,57 +57,30 @@
     <t>BS</t>
   </si>
   <si>
-    <t>FoodWasteBuyer1</t>
-  </si>
-  <si>
-    <t>FoodWasteBuyer2</t>
-  </si>
-  <si>
     <t>FoodWasteSeller2</t>
   </si>
   <si>
     <t>FoodWasteSeller1</t>
   </si>
   <si>
-    <t>138600</t>
-  </si>
-  <si>
-    <t>138601</t>
-  </si>
-  <si>
     <t>639460</t>
   </si>
   <si>
     <t>638996</t>
   </si>
   <si>
-    <t>1.3053214796692</t>
-  </si>
-  <si>
-    <t>1.30473601105044</t>
-  </si>
-  <si>
     <t>1.32675931049981</t>
   </si>
   <si>
     <t>1.32454054326825</t>
   </si>
   <si>
-    <t>103.773948937801</t>
-  </si>
-  <si>
-    <t>103.773991794709</t>
-  </si>
-  <si>
     <t>103.655123261088</t>
   </si>
   <si>
     <t>103.639491831506</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -107,6 +91,9 @@
   </si>
   <si>
     <t>delivery_fee</t>
+  </si>
+  <si>
+    <t>invest_cost</t>
   </si>
 </sst>
 </file>
@@ -487,7 +474,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -500,22 +487,27 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>1</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>2</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4">
-        <v>262</v>
+      <c r="A4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5">
-        <v>261</v>
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -525,7 +517,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -536,99 +528,59 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>1</v>
+        <v>262</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>2</v>
+        <v>261</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>262</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>261</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
         <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -652,13 +604,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -702,7 +654,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -716,38 +668,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>90</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -757,59 +681,66 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>262</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>261</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -819,13 +750,58 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>30000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -841,37 +817,127 @@
       <c r="E1" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
+        <v>262</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>261</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="D1" s="1">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>262</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>262</v>
-      </c>
-      <c r="B4">
-        <v>16.157</v>
-      </c>
-      <c r="C4">
-        <v>16.099</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
         <v>261</v>
       </c>
-      <c r="B5">
-        <v>18.131</v>
-      </c>
-      <c r="C5">
-        <v>18.073</v>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>